<commit_message>
Adjustment to driver manager automatic Chrome version
</commit_message>
<xml_diff>
--- a/TabelaTeste.xlsx
+++ b/TabelaTeste.xlsx
@@ -1693,7 +1693,7 @@
         <v>90.15000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>68.5</v>
+        <v>85.5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1701,7 +1701,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>78.75</v>
+        <v>78.76000000000001</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
         <v>168</v>
       </c>
       <c r="F4" t="n">
-        <v>189.9</v>
+        <v>189.91</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1794,10 +1794,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>149.9</v>
+        <v>159.9</v>
       </c>
       <c r="D5" t="n">
-        <v>149.9</v>
+        <v>159.9</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1805,14 +1805,14 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>141.45</v>
+        <v>137.66</v>
       </c>
       <c r="G5" t="n">
         <v>198</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1835,7 +1835,7 @@
         <v>57.9</v>
       </c>
       <c r="F6" t="n">
-        <v>59.75</v>
+        <v>59.76</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1933,7 +1933,7 @@
         <v>289.9</v>
       </c>
       <c r="F9" t="n">
-        <v>379.9</v>
+        <v>379.91</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1956,7 +1956,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>219.9</v>
+        <v>260.53</v>
       </c>
       <c r="D10" t="n">
         <v>395.5</v>
@@ -1965,7 +1965,7 @@
         <v>198</v>
       </c>
       <c r="F10" t="n">
-        <v>427.4</v>
+        <v>427.41</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -1988,10 +1988,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>167.9</v>
+        <v>169.9</v>
       </c>
       <c r="D11" t="n">
-        <v>159.9</v>
+        <v>169.9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>151.9</v>
+        <v>144.9</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -2042,7 +2042,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26.91</v>
+        <v>25.9</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -2105,7 +2105,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>52.15</v>
+        <v>55.01</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>99.90000000000001</v>
+        <v>19.2</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -2164,7 +2164,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>169.97</v>
+        <v>161.47</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -2175,14 +2175,14 @@
         <v>61.9</v>
       </c>
       <c r="F16" t="n">
-        <v>211.75</v>
+        <v>243.9</v>
       </c>
       <c r="G16" t="n">
         <v>599</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
     </row>
@@ -28652,7 +28652,7 @@
       </c>
       <c r="D2" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -28675,7 +28675,7 @@
       </c>
       <c r="D3" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -28698,7 +28698,7 @@
       </c>
       <c r="D4" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -28717,11 +28717,11 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>149.9</v>
+        <v>159.9</v>
       </c>
       <c r="D5" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -28744,7 +28744,7 @@
       </c>
       <c r="D6" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -28767,7 +28767,7 @@
       </c>
       <c r="D7" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -28790,7 +28790,7 @@
       </c>
       <c r="D8" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -28813,7 +28813,7 @@
       </c>
       <c r="D9" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -28832,11 +28832,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>219.9</v>
+        <v>260.53</v>
       </c>
       <c r="D10" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -28855,11 +28855,11 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>167.9</v>
+        <v>169.9</v>
       </c>
       <c r="D11" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -28882,7 +28882,7 @@
       </c>
       <c r="D12" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -28901,11 +28901,11 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26.91</v>
+        <v>25.9</v>
       </c>
       <c r="D13" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -28928,7 +28928,7 @@
       </c>
       <c r="D14" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -28947,11 +28947,11 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>99.90000000000001</v>
+        <v>19.2</v>
       </c>
       <c r="D15" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -28970,11 +28970,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>169.97</v>
+        <v>161.47</v>
       </c>
       <c r="D16" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -28993,11 +28993,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>68.5</v>
+        <v>85.5</v>
       </c>
       <c r="D17" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -29020,7 +29020,7 @@
       </c>
       <c r="D18" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -29039,11 +29039,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>149.9</v>
+        <v>159.9</v>
       </c>
       <c r="D19" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -29066,7 +29066,7 @@
       </c>
       <c r="D20" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -29089,7 +29089,7 @@
       </c>
       <c r="D21" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -29112,7 +29112,7 @@
       </c>
       <c r="D22" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -29135,7 +29135,7 @@
       </c>
       <c r="D23" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -29158,7 +29158,7 @@
       </c>
       <c r="D24" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -29177,11 +29177,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>159.9</v>
+        <v>169.9</v>
       </c>
       <c r="D25" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -29204,7 +29204,7 @@
       </c>
       <c r="D26" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -29227,7 +29227,7 @@
       </c>
       <c r="D27" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -29250,7 +29250,7 @@
       </c>
       <c r="D28" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -29273,7 +29273,7 @@
       </c>
       <c r="D29" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -29296,7 +29296,7 @@
       </c>
       <c r="D30" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -29319,7 +29319,7 @@
       </c>
       <c r="D31" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -29342,7 +29342,7 @@
       </c>
       <c r="D32" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -29365,7 +29365,7 @@
       </c>
       <c r="D33" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -29384,11 +29384,11 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>78.75</v>
+        <v>78.76000000000001</v>
       </c>
       <c r="D34" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -29407,11 +29407,11 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>189.9</v>
+        <v>189.91</v>
       </c>
       <c r="D35" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -29430,11 +29430,11 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>141.45</v>
+        <v>137.66</v>
       </c>
       <c r="D36" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -29453,11 +29453,11 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>59.75</v>
+        <v>59.76</v>
       </c>
       <c r="D37" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -29480,7 +29480,7 @@
       </c>
       <c r="D38" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -29499,11 +29499,11 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>379.9</v>
+        <v>379.91</v>
       </c>
       <c r="D39" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -29522,11 +29522,11 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>427.4</v>
+        <v>427.41</v>
       </c>
       <c r="D40" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -29545,11 +29545,11 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>151.9</v>
+        <v>144.9</v>
       </c>
       <c r="D41" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -29572,7 +29572,7 @@
       </c>
       <c r="D42" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -29591,11 +29591,11 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>52.15</v>
+        <v>55.01</v>
       </c>
       <c r="D43" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -29614,11 +29614,11 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>211.75</v>
+        <v>243.9</v>
       </c>
       <c r="D44" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -29641,7 +29641,7 @@
       </c>
       <c r="D45" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -29664,7 +29664,7 @@
       </c>
       <c r="D46" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -29687,7 +29687,7 @@
       </c>
       <c r="D47" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -29710,7 +29710,7 @@
       </c>
       <c r="D48" s="49" t="inlineStr">
         <is>
-          <t>14/11/24</t>
+          <t>27/11/24</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">

</xml_diff>